<commit_message>
rto month state  company script
</commit_message>
<xml_diff>
--- a/paygrid1.xlsx
+++ b/paygrid1.xlsx
@@ -148,9 +148,6 @@
     <t xml:space="preserve">Private Car Package Policy</t>
   </si>
   <si>
-    <t xml:space="preserve">Non Petrol- Diesel, CNG,LPG</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comprehensive &amp; SAOD</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve">pqr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bajaj life line</t>
   </si>
   <si>
     <t xml:space="preserve">Life Insurance</t>
@@ -229,12 +229,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -270,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,6 +302,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -300,6 +319,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF999999"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -417,13 +496,14 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.17"/>
   </cols>
   <sheetData>
@@ -469,13 +549,13 @@
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -505,7 +585,7 @@
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -541,7 +621,7 @@
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -577,7 +657,7 @@
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -613,7 +693,7 @@
       <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -649,14 +729,14 @@
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>16</v>
@@ -665,13 +745,13 @@
         <v>38</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K7" s="1" t="n">
         <f aca="false">I7*90/100</f>
@@ -680,12 +760,12 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="1" t="s">

</xml_diff>

<commit_message>
view payout upload payout done with base templates
</commit_message>
<xml_diff>
--- a/paygrid1.xlsx
+++ b/paygrid1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t xml:space="preserve">company</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">agent_payout</t>
   </si>
   <si>
-    <t xml:space="preserve">hdfc</t>
+    <t xml:space="preserve">Bajaj</t>
   </si>
   <si>
     <t xml:space="preserve">Motor Insurance</t>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">abc</t>
   </si>
   <si>
+    <t xml:space="preserve">HDFC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Two Wheeler Liability Policy</t>
   </si>
   <si>
@@ -115,7 +118,7 @@
     <t xml:space="preserve">ghi</t>
   </si>
   <si>
-    <t xml:space="preserve">bajaj</t>
+    <t xml:space="preserve">Bajaj </t>
   </si>
   <si>
     <t xml:space="preserve">Scooter without CPA</t>
@@ -179,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -213,6 +216,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -285,7 +293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,6 +315,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -496,7 +508,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -580,16 +592,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>15</v>
@@ -598,16 +610,16 @@
         <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" s="1" t="n">
         <f aca="false">I3*90/100</f>
@@ -616,34 +628,34 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>17</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K4" s="1" t="n">
         <f aca="false">I4*90/100</f>
@@ -651,17 +663,17 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>31</v>
+      <c r="A5" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
@@ -673,106 +685,106 @@
         <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>15.5</v>
+        <v>18</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K5" s="1" t="n">
         <f aca="false">I5*90/100</f>
-        <v>13.95</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>31</v>
+      <c r="A6" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K6" s="1" t="n">
         <f aca="false">I6*90/100</f>
-        <v>18</v>
+        <v>17.1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>31</v>
+      <c r="A7" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K7" s="1" t="n">
         <f aca="false">I7*90/100</f>
-        <v>17.1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>16</v>
@@ -784,14 +796,14 @@
         <v>18</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K8" s="1" t="n">
         <f aca="false">I8*90/100</f>
-        <v>13.5</v>
+        <v>18.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>